<commit_message>
Working on new airSpace class.
</commit_message>
<xml_diff>
--- a/PHX lat and long converter1.xlsx
+++ b/PHX lat and long converter1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e352454\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e352454\dev\Projects\pdla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5457D3D5-D5E0-4524-B2E8-34B2E3697555}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395EA3E7-9FF6-4DCE-85BF-D67FF090F8EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{51E1969C-4A2B-42C5-88CD-02131A8D2726}"/>
   </bookViews>
@@ -103,12 +103,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -123,10 +135,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D17263-1184-4F45-8A48-E2A233BF3566}">
-  <dimension ref="D4:K23"/>
+  <dimension ref="C4:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,31 +470,31 @@
     <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G4">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G5" s="1">
-        <v>33.434170000000002</v>
+        <v>33.267429</v>
       </c>
       <c r="H5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <v>-111.730479</v>
+      </c>
+      <c r="H6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="G6" s="1">
-        <v>-112.01167</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G7">
         <v>24901</v>
       </c>
@@ -486,7 +502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G8">
         <f>G7/360</f>
         <v>69.169444444444451</v>
@@ -495,16 +511,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G9">
         <f>G7*COS(G5*2*PI()/360)/360</f>
-        <v>57.723244636141729</v>
+        <v>57.833909542384923</v>
       </c>
       <c r="H9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G10">
         <f>1/G8</f>
         <v>1.4457250712822776E-2</v>
@@ -513,23 +529,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G11">
         <f>1/G9</f>
-        <v>1.7324043482023516E-2</v>
+        <v>1.7290894008594158E-2</v>
       </c>
       <c r="H11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="F13" s="2">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f>G4*G11</f>
+        <v>0.55330860827501305</v>
+      </c>
+      <c r="D13">
+        <f>G4*G10</f>
+        <v>0.46263202281032884</v>
+      </c>
+      <c r="F13" s="4">
         <f>G5+G4*G10</f>
-        <v>33.867887521384688</v>
-      </c>
-      <c r="G13" s="2">
+        <v>33.730061022810325</v>
+      </c>
+      <c r="G13" s="4">
         <f>G6-G4*G11</f>
-        <v>-112.5313913044607</v>
+        <v>-112.28378760827502</v>
       </c>
       <c r="H13" t="s">
         <v>10</v>
@@ -537,18 +561,18 @@
       <c r="I13" t="s">
         <v>11</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
       <c r="F14" s="2">
         <f>G5+G4*G10</f>
-        <v>33.867887521384688</v>
+        <v>33.730061022810325</v>
       </c>
       <c r="G14" s="2">
         <f>G6+G4*G11</f>
-        <v>-111.49194869553929</v>
+        <v>-111.17717039172499</v>
       </c>
       <c r="H14" t="s">
         <v>10</v>
@@ -560,14 +584,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="F15" s="2">
         <f>G5-G4*G10</f>
-        <v>33.000452478615315</v>
+        <v>32.804796977189675</v>
       </c>
       <c r="G15" s="2">
         <f>G6-G4*G11</f>
-        <v>-112.5313913044607</v>
+        <v>-112.28378760827502</v>
       </c>
       <c r="H15" t="s">
         <v>10</v>
@@ -579,17 +603,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D16" s="1">
-        <v>33.267429</v>
-      </c>
-      <c r="F16" s="2">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F16" s="4">
         <f>G5-G4*G10</f>
-        <v>33.000452478615315</v>
-      </c>
-      <c r="G16" s="2">
+        <v>32.804796977189675</v>
+      </c>
+      <c r="G16" s="4">
         <f>G6+G4*G11</f>
-        <v>-111.49194869553929</v>
+        <v>-111.17717039172499</v>
       </c>
       <c r="H16" t="s">
         <v>10</v>
@@ -597,76 +618,83 @@
       <c r="I16" t="s">
         <v>11</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D17">
-        <f>D16/360*2*PI()</f>
-        <v>0.58062616972344472</v>
-      </c>
-      <c r="F17" s="2">
+      <c r="P16">
+        <f>30/8</f>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="F18" s="5">
         <f>G5</f>
-        <v>33.434170000000002</v>
-      </c>
-      <c r="G17" s="2">
+        <v>33.267429</v>
+      </c>
+      <c r="G18" s="5">
         <f>G6</f>
-        <v>-112.01167</v>
-      </c>
-      <c r="H17" t="s">
+        <v>-111.730479</v>
+      </c>
+      <c r="H18" t="s">
         <v>9</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I18" t="s">
         <v>12</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K18" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D18">
-        <f>COS(D17)</f>
-        <v>0.83611932995697258</v>
-      </c>
-    </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D19">
-        <f>D18*G7</f>
-        <v>20820.207435258573</v>
-      </c>
-    </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D20">
-        <f>D19/360</f>
-        <v>57.833909542384923</v>
+      <c r="D20" s="1">
+        <v>33.267429</v>
       </c>
       <c r="F20" s="2">
         <f>MIN(F13:F16)</f>
-        <v>33.000452478615315</v>
+        <v>32.804796977189675</v>
       </c>
       <c r="G20" s="2">
         <f>MIN(G13:G16)</f>
-        <v>-112.5313913044607</v>
+        <v>-112.28378760827502</v>
       </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f>D20/360*2*PI()</f>
+        <v>0.58062616972344472</v>
+      </c>
       <c r="F21" s="2">
         <f>MAX(F13:F16)</f>
-        <v>33.867887521384688</v>
+        <v>33.730061022810325</v>
       </c>
       <c r="G21" s="2">
         <f>MAX(G13:G16)</f>
-        <v>-111.49194869553929</v>
+        <v>-111.17717039172499</v>
+      </c>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f>COS(D21)</f>
+        <v>0.83611932995697258</v>
       </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <f>D22*G7</f>
+        <v>20820.207435258573</v>
+      </c>
       <c r="F23" t="s">
         <v>17</v>
       </c>
       <c r="G23" t="str">
-        <f>_xlfn.CONCAT("(",F20,", ",F21,", ",G20,", ",G21,")")</f>
-        <v>(33.0004524786153, 33.8678875213847, -112.531391304461, -111.491948695539)</v>
+        <f>_xlfn.CONCAT("(",G20,", ",F21,", ",G21,", ",F20,")")</f>
+        <v>(-112.283787608275, 33.7300610228103, -111.177170391725, 32.8047969771897)</v>
+      </c>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f>D23/360</f>
+        <v>57.833909542384923</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Debugging creation of cells in airspace.
</commit_message>
<xml_diff>
--- a/PHX lat and long converter1.xlsx
+++ b/PHX lat and long converter1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e352454\dev\Projects\pdla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395EA3E7-9FF6-4DCE-85BF-D67FF090F8EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA42E161-2C21-4DBB-A0FD-8EA59852DD68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" xr2:uid="{51E1969C-4A2B-42C5-88CD-02131A8D2726}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Circumference of Earth (mi)</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>bbox</t>
+  </si>
+  <si>
+    <t>CTR</t>
+  </si>
+  <si>
+    <t>cellCoord</t>
+  </si>
+  <si>
+    <t>newCTR</t>
   </si>
 </sst>
 </file>
@@ -123,7 +132,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -131,11 +140,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -143,6 +167,10 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D17263-1184-4F45-8A48-E2A233BF3566}">
-  <dimension ref="C4:P24"/>
+  <dimension ref="C4:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +498,7 @@
     <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
       <c r="G4">
         <v>32</v>
       </c>
@@ -478,7 +506,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
       <c r="G5" s="1">
         <v>33.267429</v>
       </c>
@@ -486,7 +514,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="G6" s="1">
         <v>-111.730479</v>
       </c>
@@ -494,7 +522,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="G7">
         <v>24901</v>
       </c>
@@ -502,7 +530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="G8">
         <f>G7/360</f>
         <v>69.169444444444451</v>
@@ -511,7 +539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="G9">
         <f>G7*COS(G5*2*PI()/360)/360</f>
         <v>57.833909542384923</v>
@@ -520,7 +548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="G10">
         <f>1/G8</f>
         <v>1.4457250712822776E-2</v>
@@ -529,7 +557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
       <c r="G11">
         <f>1/G9</f>
         <v>1.7290894008594158E-2</v>
@@ -538,7 +566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C13">
         <f>G4*G11</f>
         <v>0.55330860827501305</v>
@@ -565,7 +593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F14" s="2">
         <f>G5+G4*G10</f>
         <v>33.730061022810325</v>
@@ -584,7 +612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F15" s="2">
         <f>G5-G4*G10</f>
         <v>32.804796977189675</v>
@@ -603,7 +631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
       <c r="F16" s="4">
         <f>G5-G4*G10</f>
         <v>32.804796977189675</v>
@@ -622,11 +650,23 @@
         <v>8</v>
       </c>
       <c r="P16">
-        <f>30/8</f>
-        <v>3.75</v>
-      </c>
-    </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+        <v>6.9163576034376603E-2</v>
+      </c>
+      <c r="Q16">
+        <f>P16/G11</f>
+        <v>3.9999999999999982</v>
+      </c>
+    </row>
+    <row r="17" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>5.7829002851291098E-2</v>
+      </c>
+      <c r="Q17">
+        <f>P17/G10</f>
+        <v>3.9999999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="4:22" x14ac:dyDescent="0.25">
       <c r="F18" s="5">
         <f>G5</f>
         <v>33.267429</v>
@@ -645,7 +685,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D20" s="1">
         <v>33.267429</v>
       </c>
@@ -658,7 +698,7 @@
         <v>-112.28378760827502</v>
       </c>
     </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D21">
         <f>D20/360*2*PI()</f>
         <v>0.58062616972344472</v>
@@ -672,13 +712,31 @@
         <v>-111.17717039172499</v>
       </c>
     </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D22">
         <f>COS(D21)</f>
         <v>0.83611932995697258</v>
       </c>
-    </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="P22" s="8">
+        <v>-112.007133304137</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>33.498745011405099</v>
+      </c>
+      <c r="R22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="T22" s="8">
+        <v>-112.04171509215401</v>
+      </c>
+      <c r="U22" s="8">
+        <v>33.527659512830802</v>
+      </c>
+      <c r="V22" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D23">
         <f>D22*G7</f>
         <v>20820.207435258573</v>
@@ -690,11 +748,105 @@
         <f>_xlfn.CONCAT("(",G20,", ",F21,", ",G21,", ",F20,")")</f>
         <v>(-112.283787608275, 33.7300610228103, -111.177170391725, 32.8047969771897)</v>
       </c>
-    </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="P23" s="8">
+        <v>-111.730479</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>33.267429</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T23" s="8">
+        <v>-112.007133304137</v>
+      </c>
+      <c r="U23" s="8">
+        <v>33.498745011405099</v>
+      </c>
+      <c r="V23" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D24">
         <f>D23/360</f>
         <v>57.833909542384923</v>
+      </c>
+      <c r="P24" s="8">
+        <f>P22-P23</f>
+        <v>-0.2766543041369971</v>
+      </c>
+      <c r="Q24" s="8">
+        <f>Q22-Q23</f>
+        <v>0.23131601140509872</v>
+      </c>
+      <c r="T24" s="8">
+        <f>T22-T23</f>
+        <v>-3.4581788017007398E-2</v>
+      </c>
+      <c r="U24" s="8">
+        <f>U22-U23</f>
+        <v>2.8914501425703065E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="P25" s="7">
+        <f>P24/$G$11</f>
+        <v>-15.999999999970537</v>
+      </c>
+      <c r="Q25" s="7">
+        <f>Q24/$G$10</f>
+        <v>15.999999999995456</v>
+      </c>
+      <c r="T25" s="7">
+        <f>T24/$G$11</f>
+        <v>-1.9999999999895368</v>
+      </c>
+      <c r="U25" s="7">
+        <f>U24/$G$10</f>
+        <v>2.0000000000039782</v>
+      </c>
+    </row>
+    <row r="30" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="T30" s="8">
+        <v>-112.007133304137</v>
+      </c>
+      <c r="U30" s="8">
+        <v>33.498745011405099</v>
+      </c>
+      <c r="V30" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="T31" s="8">
+        <v>-111.97255151612001</v>
+      </c>
+      <c r="U31" s="8">
+        <v>33.585488515682101</v>
+      </c>
+      <c r="V31" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="T32" s="8">
+        <f>T31-T30</f>
+        <v>3.4581788016993187E-2</v>
+      </c>
+      <c r="U32" s="8">
+        <f>U31-U30</f>
+        <v>8.6743504277002614E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="20:21" x14ac:dyDescent="0.25">
+      <c r="T33" s="7">
+        <f>T32/$G$11</f>
+        <v>1.999999999988715</v>
+      </c>
+      <c r="U33" s="7">
+        <f>U32/$G$10</f>
+        <v>6.0000000000045626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>